<commit_message>
data entry and cleaning code
</commit_message>
<xml_diff>
--- a/data/Subsampling_weights.xlsx
+++ b/data/Subsampling_weights.xlsx
@@ -20,13 +20,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
+    <t>Core_No</t>
+  </si>
+  <si>
+    <t>Moisture_perc</t>
+  </si>
+  <si>
     <t>Core</t>
   </si>
   <si>
-    <t>Core_No</t>
-  </si>
-  <si>
-    <t>TC_g</t>
+    <t>TC_targetOD_g</t>
   </si>
   <si>
     <t>Tray_No</t>
@@ -47,28 +50,7 @@
     <t>DrySoil_g</t>
   </si>
   <si>
-    <t>Moisture_perc</t>
-  </si>
-  <si>
-    <t>WSOC_g</t>
-  </si>
-  <si>
-    <t>Aggregate_g</t>
-  </si>
-  <si>
-    <t>Bulk_g</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Initials</t>
-  </si>
-  <si>
-    <t>TC_targetOD_g</t>
-  </si>
-  <si>
-    <t>TARGET</t>
+    <t>TC_g</t>
   </si>
   <si>
     <t>TC_targetMoist_g</t>
@@ -86,13 +68,31 @@
     <t>WSOC_weighed_g</t>
   </si>
   <si>
+    <t>WSOC_g</t>
+  </si>
+  <si>
+    <t>Aggregate_g</t>
+  </si>
+  <si>
+    <t>Bulk_g</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
     <t>Aggregate_targetMoist_g</t>
+  </si>
+  <si>
+    <t>Initials</t>
   </si>
   <si>
     <t>Aggregate_weighed_g</t>
   </si>
   <si>
     <t>Bulk_weighed_g</t>
+  </si>
+  <si>
+    <t>TARGET</t>
   </si>
   <si>
     <t>27-ish</t>
@@ -124,9 +124,8 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
       <sz val="12.0"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -134,17 +133,18 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <b/>
       <sz val="12.0"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font/>
     <font>
       <b/>
       <sz val="12.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -231,54 +231,54 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="3" fontId="1" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="9" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="9" fontId="6" numFmtId="4" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="7" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf borderId="1" fillId="9" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="6" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf borderId="1" fillId="9" fontId="6" numFmtId="4" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="1" fillId="3" fontId="7" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
@@ -287,12 +287,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="7" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="1" fillId="9" fontId="6" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="1" fillId="4" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -534,197 +534,197 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>131.0</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <f t="shared" ref="F2:F11" si="1">D2-C2</f>
         <v>0</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <f t="shared" ref="G2:G11" si="2">E2-C2</f>
         <v>0</v>
       </c>
-      <c r="H2" s="7" t="str">
+      <c r="H2" s="6" t="str">
         <f t="shared" ref="H2:H11" si="3">((F2-G2)/G2)*100</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>132.0</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H3" s="7" t="str">
+      <c r="H3" s="6" t="str">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="2">
+      <c r="A4" s="3">
         <v>133.0</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H4" s="7" t="str">
+      <c r="H4" s="6" t="str">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="2">
+      <c r="A5" s="3">
         <v>134.0</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H5" s="7" t="str">
+      <c r="H5" s="6" t="str">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="2">
+      <c r="A6" s="3">
         <v>135.0</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H6" s="7" t="str">
+      <c r="H6" s="6" t="str">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="2">
+      <c r="A7" s="3">
         <v>136.0</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H7" s="7" t="str">
+      <c r="H7" s="6" t="str">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="2">
+      <c r="A8" s="3">
         <v>137.0</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H8" s="7" t="str">
+      <c r="H8" s="6" t="str">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="2">
+      <c r="A9" s="3">
         <v>138.0</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H9" s="7" t="str">
+      <c r="H9" s="6" t="str">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="2">
+      <c r="A10" s="3">
         <v>139.0</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H10" s="7" t="str">
+      <c r="H10" s="6" t="str">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="2">
+      <c r="A11" s="3">
         <v>140.0</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H11" s="7" t="str">
+      <c r="H11" s="6" t="str">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
@@ -1742,7 +1742,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="7.22"/>
     <col customWidth="1" min="2" max="2" width="11.44"/>
-    <col customWidth="1" min="3" max="3" width="11.33"/>
+    <col customWidth="1" min="3" max="3" width="11.89"/>
     <col customWidth="1" min="4" max="4" width="13.78"/>
     <col customWidth="1" min="5" max="5" width="11.44"/>
     <col customWidth="1" min="6" max="6" width="14.56"/>
@@ -1755,52 +1755,52 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="9" t="s">
+      <c r="I1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="14" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="16">
+      <c r="A2" s="15">
         <f>moisture!A2</f>
         <v>131</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="16">
         <v>70.0</v>
       </c>
-      <c r="C2" s="19">
+      <c r="C2" s="17">
         <v>3.0</v>
       </c>
-      <c r="D2" s="20">
+      <c r="D2" s="19">
         <f>C2*(($B2/100)+1)</f>
         <v>5.1</v>
       </c>
@@ -1813,14 +1813,14 @@
         <v>6.8</v>
       </c>
       <c r="H2" s="24"/>
-      <c r="I2" s="12">
+      <c r="I2" s="11">
         <v>10.0</v>
       </c>
       <c r="J2" s="25"/>
       <c r="K2" s="26"/>
     </row>
     <row r="3">
-      <c r="A3" s="16">
+      <c r="A3" s="15">
         <f>moisture!A3</f>
         <v>132</v>
       </c>
@@ -1835,7 +1835,7 @@
       <c r="K3" s="26"/>
     </row>
     <row r="4">
-      <c r="A4" s="16">
+      <c r="A4" s="15">
         <f>moisture!A4</f>
         <v>133</v>
       </c>
@@ -1850,7 +1850,7 @@
       <c r="K4" s="26"/>
     </row>
     <row r="5">
-      <c r="A5" s="16">
+      <c r="A5" s="15">
         <f>moisture!A5</f>
         <v>134</v>
       </c>
@@ -1865,7 +1865,7 @@
       <c r="K5" s="26"/>
     </row>
     <row r="6">
-      <c r="A6" s="16">
+      <c r="A6" s="15">
         <f>moisture!A6</f>
         <v>135</v>
       </c>
@@ -1880,7 +1880,7 @@
       <c r="K6" s="26"/>
     </row>
     <row r="7">
-      <c r="A7" s="16">
+      <c r="A7" s="15">
         <f>moisture!A7</f>
         <v>136</v>
       </c>
@@ -1895,7 +1895,7 @@
       <c r="K7" s="26"/>
     </row>
     <row r="8">
-      <c r="A8" s="16">
+      <c r="A8" s="15">
         <f>moisture!A8</f>
         <v>137</v>
       </c>
@@ -1910,7 +1910,7 @@
       <c r="K8" s="26"/>
     </row>
     <row r="9">
-      <c r="A9" s="16">
+      <c r="A9" s="15">
         <f>moisture!A9</f>
         <v>138</v>
       </c>
@@ -1925,7 +1925,7 @@
       <c r="K9" s="26"/>
     </row>
     <row r="10">
-      <c r="A10" s="16">
+      <c r="A10" s="15">
         <f>moisture!A10</f>
         <v>139</v>
       </c>
@@ -1940,7 +1940,7 @@
       <c r="K10" s="26"/>
     </row>
     <row r="11">
-      <c r="A11" s="16">
+      <c r="A11" s="15">
         <f>moisture!A11</f>
         <v>140</v>
       </c>
@@ -1955,7 +1955,7 @@
       <c r="K11" s="26"/>
     </row>
     <row r="12">
-      <c r="A12" s="16" t="str">
+      <c r="A12" s="15" t="str">
         <f>moisture!A12</f>
         <v/>
       </c>
@@ -12778,269 +12778,269 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
+      <c r="C1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="3">
+      <c r="A2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="9">
         <v>3.0</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="14">
         <v>4.0</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="9">
         <v>10.0</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="15">
+      <c r="A3" s="18">
         <v>1.0</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="20">
         <v>3.1</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="20">
         <v>3.987</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="20">
         <v>9.904</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="20">
         <v>27.91</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
-      <c r="V3" s="15"/>
-      <c r="W3" s="15"/>
-      <c r="X3" s="15"/>
-      <c r="Y3" s="15"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="18"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
+      <c r="Y3" s="18"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="15">
+      <c r="A4" s="18">
         <v>2.0</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="20">
         <v>3.167</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="20">
         <v>4.023</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="20">
         <v>9.925</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="20">
         <v>27.974</v>
       </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="15"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="18"/>
+      <c r="W4" s="18"/>
+      <c r="X4" s="18"/>
+      <c r="Y4" s="18"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="15">
+      <c r="A5" s="18">
         <v>3.0</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="20">
         <v>3.054</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="20">
         <v>3.945</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="20">
         <v>10.096</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="18"/>
+      <c r="U5" s="18"/>
+      <c r="V5" s="18"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="18"/>
+      <c r="Y5" s="18"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="15">
+      <c r="A6" s="18">
         <v>4.0</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="20">
         <v>3.112</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="20">
         <v>3.973</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="20">
         <v>9.983</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="20">
         <v>27.87</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="15"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="18"/>
+      <c r="V6" s="18"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="18"/>
+      <c r="Y6" s="18"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="15">
+      <c r="A7" s="18">
         <v>5.0</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="20">
         <v>3.126</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="20">
         <v>3.944</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="20">
         <v>10.09</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="20">
         <v>27.24</v>
       </c>
       <c r="F7" s="32">
         <v>43746.0</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
-      <c r="T7" s="15"/>
-      <c r="U7" s="15"/>
-      <c r="V7" s="15"/>
-      <c r="W7" s="15"/>
-      <c r="X7" s="15"/>
-      <c r="Y7" s="15"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="18"/>
+      <c r="T7" s="18"/>
+      <c r="U7" s="18"/>
+      <c r="V7" s="18"/>
+      <c r="W7" s="18"/>
+      <c r="X7" s="18"/>
+      <c r="Y7" s="18"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="33">
@@ -13834,193 +13834,193 @@
       <c r="E63" s="40"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="15">
+      <c r="A64" s="18">
         <v>56.0</v>
       </c>
-      <c r="B64" s="17">
+      <c r="B64" s="20">
         <v>2.95</v>
       </c>
-      <c r="C64" s="17">
+      <c r="C64" s="20">
         <v>4.051</v>
       </c>
-      <c r="D64" s="17">
+      <c r="D64" s="20">
         <v>10.047</v>
       </c>
-      <c r="E64" s="17">
+      <c r="E64" s="20">
         <v>21.515</v>
       </c>
-      <c r="F64" s="15"/>
-      <c r="G64" s="15"/>
-      <c r="H64" s="15"/>
-      <c r="I64" s="15"/>
-      <c r="J64" s="15"/>
-      <c r="K64" s="15"/>
-      <c r="L64" s="15"/>
-      <c r="M64" s="15"/>
-      <c r="N64" s="15"/>
-      <c r="O64" s="15"/>
-      <c r="P64" s="15"/>
-      <c r="Q64" s="15"/>
-      <c r="R64" s="15"/>
-      <c r="S64" s="15"/>
-      <c r="T64" s="15"/>
-      <c r="U64" s="15"/>
-      <c r="V64" s="15"/>
-      <c r="W64" s="15"/>
-      <c r="X64" s="15"/>
-      <c r="Y64" s="15"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="18"/>
+      <c r="I64" s="18"/>
+      <c r="J64" s="18"/>
+      <c r="K64" s="18"/>
+      <c r="L64" s="18"/>
+      <c r="M64" s="18"/>
+      <c r="N64" s="18"/>
+      <c r="O64" s="18"/>
+      <c r="P64" s="18"/>
+      <c r="Q64" s="18"/>
+      <c r="R64" s="18"/>
+      <c r="S64" s="18"/>
+      <c r="T64" s="18"/>
+      <c r="U64" s="18"/>
+      <c r="V64" s="18"/>
+      <c r="W64" s="18"/>
+      <c r="X64" s="18"/>
+      <c r="Y64" s="18"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="15">
+      <c r="A65" s="18">
         <v>57.0</v>
       </c>
-      <c r="B65" s="17">
+      <c r="B65" s="20">
         <v>3.07</v>
       </c>
-      <c r="C65" s="17">
+      <c r="C65" s="20">
         <v>3.989</v>
       </c>
-      <c r="D65" s="17">
+      <c r="D65" s="20">
         <v>10.022</v>
       </c>
-      <c r="E65" s="17">
+      <c r="E65" s="20">
         <v>15.52</v>
       </c>
-      <c r="F65" s="15"/>
-      <c r="G65" s="15"/>
-      <c r="H65" s="15"/>
-      <c r="I65" s="15"/>
-      <c r="J65" s="15"/>
-      <c r="K65" s="15"/>
-      <c r="L65" s="15"/>
-      <c r="M65" s="15"/>
-      <c r="N65" s="15"/>
-      <c r="O65" s="15"/>
-      <c r="P65" s="15"/>
-      <c r="Q65" s="15"/>
-      <c r="R65" s="15"/>
-      <c r="S65" s="15"/>
-      <c r="T65" s="15"/>
-      <c r="U65" s="15"/>
-      <c r="V65" s="15"/>
-      <c r="W65" s="15"/>
-      <c r="X65" s="15"/>
-      <c r="Y65" s="15"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="18"/>
+      <c r="I65" s="18"/>
+      <c r="J65" s="18"/>
+      <c r="K65" s="18"/>
+      <c r="L65" s="18"/>
+      <c r="M65" s="18"/>
+      <c r="N65" s="18"/>
+      <c r="O65" s="18"/>
+      <c r="P65" s="18"/>
+      <c r="Q65" s="18"/>
+      <c r="R65" s="18"/>
+      <c r="S65" s="18"/>
+      <c r="T65" s="18"/>
+      <c r="U65" s="18"/>
+      <c r="V65" s="18"/>
+      <c r="W65" s="18"/>
+      <c r="X65" s="18"/>
+      <c r="Y65" s="18"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="15">
+      <c r="A66" s="18">
         <v>58.0</v>
       </c>
-      <c r="B66" s="17">
+      <c r="B66" s="20">
         <v>3.01</v>
       </c>
-      <c r="C66" s="17">
+      <c r="C66" s="20">
         <v>4.016</v>
       </c>
-      <c r="D66" s="17">
+      <c r="D66" s="20">
         <v>10.032</v>
       </c>
-      <c r="E66" s="17">
+      <c r="E66" s="20">
         <v>20.73</v>
       </c>
-      <c r="F66" s="15"/>
-      <c r="G66" s="15"/>
-      <c r="H66" s="15"/>
-      <c r="I66" s="15"/>
-      <c r="J66" s="15"/>
-      <c r="K66" s="15"/>
-      <c r="L66" s="15"/>
-      <c r="M66" s="15"/>
-      <c r="N66" s="15"/>
-      <c r="O66" s="15"/>
-      <c r="P66" s="15"/>
-      <c r="Q66" s="15"/>
-      <c r="R66" s="15"/>
-      <c r="S66" s="15"/>
-      <c r="T66" s="15"/>
-      <c r="U66" s="15"/>
-      <c r="V66" s="15"/>
-      <c r="W66" s="15"/>
-      <c r="X66" s="15"/>
-      <c r="Y66" s="15"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="18"/>
+      <c r="I66" s="18"/>
+      <c r="J66" s="18"/>
+      <c r="K66" s="18"/>
+      <c r="L66" s="18"/>
+      <c r="M66" s="18"/>
+      <c r="N66" s="18"/>
+      <c r="O66" s="18"/>
+      <c r="P66" s="18"/>
+      <c r="Q66" s="18"/>
+      <c r="R66" s="18"/>
+      <c r="S66" s="18"/>
+      <c r="T66" s="18"/>
+      <c r="U66" s="18"/>
+      <c r="V66" s="18"/>
+      <c r="W66" s="18"/>
+      <c r="X66" s="18"/>
+      <c r="Y66" s="18"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="15">
+      <c r="A67" s="18">
         <v>59.0</v>
       </c>
-      <c r="B67" s="17">
+      <c r="B67" s="20">
         <v>2.971</v>
       </c>
-      <c r="C67" s="17">
+      <c r="C67" s="20">
         <v>3.998</v>
       </c>
-      <c r="D67" s="17">
+      <c r="D67" s="20">
         <v>10.06</v>
       </c>
-      <c r="E67" s="17">
+      <c r="E67" s="20">
         <v>21.653</v>
       </c>
-      <c r="F67" s="15"/>
-      <c r="G67" s="15"/>
-      <c r="H67" s="15"/>
-      <c r="I67" s="15"/>
-      <c r="J67" s="15"/>
-      <c r="K67" s="15"/>
-      <c r="L67" s="15"/>
-      <c r="M67" s="15"/>
-      <c r="N67" s="15"/>
-      <c r="O67" s="15"/>
-      <c r="P67" s="15"/>
-      <c r="Q67" s="15"/>
-      <c r="R67" s="15"/>
-      <c r="S67" s="15"/>
-      <c r="T67" s="15"/>
-      <c r="U67" s="15"/>
-      <c r="V67" s="15"/>
-      <c r="W67" s="15"/>
-      <c r="X67" s="15"/>
-      <c r="Y67" s="15"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="18"/>
+      <c r="I67" s="18"/>
+      <c r="J67" s="18"/>
+      <c r="K67" s="18"/>
+      <c r="L67" s="18"/>
+      <c r="M67" s="18"/>
+      <c r="N67" s="18"/>
+      <c r="O67" s="18"/>
+      <c r="P67" s="18"/>
+      <c r="Q67" s="18"/>
+      <c r="R67" s="18"/>
+      <c r="S67" s="18"/>
+      <c r="T67" s="18"/>
+      <c r="U67" s="18"/>
+      <c r="V67" s="18"/>
+      <c r="W67" s="18"/>
+      <c r="X67" s="18"/>
+      <c r="Y67" s="18"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="15">
+      <c r="A68" s="18">
         <v>60.0</v>
       </c>
-      <c r="B68" s="17">
+      <c r="B68" s="20">
         <v>3.063</v>
       </c>
-      <c r="C68" s="17">
+      <c r="C68" s="20">
         <v>4.008</v>
       </c>
-      <c r="D68" s="17">
+      <c r="D68" s="20">
         <v>10.05</v>
       </c>
-      <c r="E68" s="17">
+      <c r="E68" s="20">
         <v>18.151</v>
       </c>
       <c r="F68" s="32">
         <v>43746.0</v>
       </c>
-      <c r="G68" s="15" t="s">
+      <c r="G68" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H68" s="15"/>
-      <c r="I68" s="15"/>
-      <c r="J68" s="15"/>
-      <c r="K68" s="15"/>
-      <c r="L68" s="15"/>
-      <c r="M68" s="15"/>
-      <c r="N68" s="15"/>
-      <c r="O68" s="15"/>
-      <c r="P68" s="15"/>
-      <c r="Q68" s="15"/>
-      <c r="R68" s="15"/>
-      <c r="S68" s="15"/>
-      <c r="T68" s="15"/>
-      <c r="U68" s="15"/>
-      <c r="V68" s="15"/>
-      <c r="W68" s="15"/>
-      <c r="X68" s="15"/>
-      <c r="Y68" s="15"/>
+      <c r="H68" s="18"/>
+      <c r="I68" s="18"/>
+      <c r="J68" s="18"/>
+      <c r="K68" s="18"/>
+      <c r="L68" s="18"/>
+      <c r="M68" s="18"/>
+      <c r="N68" s="18"/>
+      <c r="O68" s="18"/>
+      <c r="P68" s="18"/>
+      <c r="Q68" s="18"/>
+      <c r="R68" s="18"/>
+      <c r="S68" s="18"/>
+      <c r="T68" s="18"/>
+      <c r="U68" s="18"/>
+      <c r="V68" s="18"/>
+      <c r="W68" s="18"/>
+      <c r="X68" s="18"/>
+      <c r="Y68" s="18"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="41">

</xml_diff>